<commit_message>
step_3 updated and reran
</commit_message>
<xml_diff>
--- a/Notebooks/results/drug_scores_DiSCoVER_only_for_all_pdx_models.xlsx
+++ b/Notebooks/results/drug_scores_DiSCoVER_only_for_all_pdx_models.xlsx
@@ -6972,7 +6972,7 @@
         <v>0.387</v>
       </c>
       <c r="G29">
-        <v>0.442</v>
+        <v>0.4429999999999999</v>
       </c>
       <c r="H29">
         <v>0.433</v>
@@ -6999,7 +6999,7 @@
         <v>0.429</v>
       </c>
       <c r="P29">
-        <v>0.394</v>
+        <v>0.393</v>
       </c>
       <c r="Q29">
         <v>0.415</v>

</xml_diff>